<commit_message>
update db and migration
</commit_message>
<xml_diff>
--- a/IMS/wwwroot/import/customer/Test_Excel.xlsx
+++ b/IMS/wwwroot/import/customer/Test_Excel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Z_STUDYYYYY\Capstone\IMS\IMS\wwwroot\import\customer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F9AD93-7ACB-4614-9B25-B502DD6A0B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2676EA4-2536-4669-A271-CD7E56B7E289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{96F0708B-C260-474A-A5B2-5271D5C263F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Fullname</t>
   </si>
@@ -81,25 +81,6 @@
 </t>
   </si>
   <si>
-    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <d:rPr>
-        <d:sz val="11"/>
-        <d:rFont val="Arial"/>
-      </d:rPr>
-      <d:t xml:space="preserve">The Email field is not a valid e-mail address._x005F_x005F_x000D_
-</d:t>
-    </d:r>
-    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-      <d:rPr>
-        <d:sz val="11"/>
-        <d:color rgb="FF000000"/>
-        <d:rFont val="Arial"/>
-      </d:rPr>
-      <d:t xml:space="preserve">The PhoneNumber field is not a valid phone number._x005F_x005F_x000D_
-</d:t>
-    </d:r>
-  </si>
-  <si>
     <t>Trần Cao Vỹ</t>
   </si>
   <si>
@@ -113,9 +94,6 @@
   </si>
   <si>
     <t>FPT</t>
-  </si>
-  <si>
-    <t>Ok</t>
   </si>
   <si>
     <t>User EXISTED</t>
@@ -167,8 +145,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,19 +188,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -544,203 +515,192 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:L6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="14.09765625" customWidth="1"/>
+    <col min="1" max="1" width="14.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.09765625" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="9.796875" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="10.19921875" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="13.69921875" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="13" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:13" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="0">
+      <c r="G2">
         <v>11111111</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>14</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3">
+        <v>124124124</v>
+      </c>
+      <c r="G3">
+        <v>22222222</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="0" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <v>741457888</v>
+      </c>
+      <c r="G4">
+        <v>33333333</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="0">
-        <v>124124124</v>
-      </c>
-      <c r="G3" s="0">
-        <v>22222222</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="M3" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="J4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="0">
-        <v>741457888</v>
-      </c>
-      <c r="G4" s="0">
-        <v>33333333</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>348479343</v>
+      </c>
+      <c r="G5">
+        <v>44444444</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="0" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="0">
-        <v>348479343</v>
-      </c>
-      <c r="G5" s="0">
-        <v>44444444</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="M5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+      <c r="C6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>744089975</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>55555555</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
+      <c r="H6" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="M6" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId13"/>
-    <hyperlink ref="B3" r:id="rId14"/>
-    <hyperlink ref="B4" r:id="rId15"/>
-    <hyperlink ref="B5" r:id="rId16"/>
-    <hyperlink ref="B6" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>